<commit_message>
chemistry update to 20190730
</commit_message>
<xml_diff>
--- a/RAnalysis/Data/Algae.cell.counts.xlsx
+++ b/RAnalysis/Data/Algae.cell.counts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjg\Documents\My_Projects\Inragenerational_thresholds_OA\RAnalysis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC50636-41E3-4F4D-A890-AE653B3D30DE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A3B886-F64F-4752-9B0C-C5F7B78E96EB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{0EBA9A0A-F69F-410F-A8FD-B5357F2350B2}"/>
+    <workbookView xWindow="4110" yWindow="1170" windowWidth="14775" windowHeight="10005" xr2:uid="{0EBA9A0A-F69F-410F-A8FD-B5357F2350B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>right on target</t>
+  </si>
+  <si>
+    <t>day 5</t>
+  </si>
+  <si>
+    <t>day 6</t>
   </si>
 </sst>
 </file>
@@ -443,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{208EABC4-C397-41D1-9A07-B15BC63CDF74}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,6 +753,166 @@
         <v>18</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>20190729</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14">
+        <v>51100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>20190729</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D15">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <v>53600</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>20190729</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="D16">
+        <v>29</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16">
+        <v>56400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>20190729</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>916000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>20190730</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18">
+        <v>56400</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>20190730</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D19">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>59200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20190730</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D20">
+        <v>29</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20190730</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21">
+        <v>462000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>